<commit_message>
p2p_parser: add zero lines in results file for months without cash flows
</commit_message>
<xml_diff>
--- a/tests/expected_results/result_test_write_results_robocash.xlsx
+++ b/tests/expected_results/result_test_write_results_robocash.xlsx
@@ -212,8 +212,8 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="D3 H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -227,8 +227,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="10" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="10" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1018" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -276,7 +276,7 @@
       <c r="E2" s="2" t="n">
         <v>1229.48</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="n">
@@ -301,7 +301,7 @@
       <c r="E3" s="2" t="n">
         <v>1408.22</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="n">
@@ -321,13 +321,13 @@
         <v>43346</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>1310.28</v>
+        <v>1408.22</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>1606.72</v>
       </c>
-      <c r="F4" s="2" t="n">
-        <v>84.33</v>
+      <c r="F4" s="0" t="n">
+        <v>-84.33</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>279.52</v>
@@ -351,7 +351,7 @@
       <c r="E5" s="2" t="n">
         <v>2083.28</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G5" s="2" t="n">
@@ -376,8 +376,8 @@
       <c r="E6" s="2" t="n">
         <v>2014.2</v>
       </c>
-      <c r="F6" s="2" t="n">
-        <v>123.83</v>
+      <c r="F6" s="0" t="n">
+        <v>-123.83</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>53.52</v>
@@ -401,7 +401,7 @@
       <c r="E7" s="2" t="n">
         <v>2039.51</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="2" t="n">
@@ -421,13 +421,13 @@
         <v>43352</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>1719.51</v>
+        <v>2039.51</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>1955.78</v>
       </c>
-      <c r="F8" s="2" t="n">
-        <v>160</v>
+      <c r="F8" s="0" t="n">
+        <v>-160</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>74.56</v>
@@ -451,7 +451,7 @@
       <c r="E9" s="2" t="n">
         <v>1970.58</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="2" t="n">
@@ -476,8 +476,8 @@
       <c r="E10" s="2" t="n">
         <v>2111.07</v>
       </c>
-      <c r="F10" s="2" t="n">
-        <v>87.1</v>
+      <c r="F10" s="0" t="n">
+        <v>-87.1</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>225.08</v>
@@ -496,13 +496,13 @@
         <v>43355</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>1654.37</v>
+        <v>2111.07</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>1882.72</v>
       </c>
-      <c r="F11" s="2" t="n">
-        <v>228.35</v>
+      <c r="F11" s="0" t="n">
+        <v>-228.35</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>0</v>
@@ -526,8 +526,8 @@
       <c r="E12" s="2" t="n">
         <v>1533</v>
       </c>
-      <c r="F12" s="2" t="n">
-        <v>428.76</v>
+      <c r="F12" s="0" t="n">
+        <v>-428.76</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>77.26</v>
@@ -551,8 +551,8 @@
       <c r="E13" s="2" t="n">
         <v>1162.86</v>
       </c>
-      <c r="F13" s="2" t="n">
-        <v>500</v>
+      <c r="F13" s="0" t="n">
+        <v>-500</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>128.29</v>
@@ -576,8 +576,8 @@
       <c r="E14" s="2" t="n">
         <v>1020.96</v>
       </c>
-      <c r="F14" s="2" t="n">
-        <v>297.3</v>
+      <c r="F14" s="0" t="n">
+        <v>-297.3</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>152.31</v>
@@ -601,8 +601,8 @@
       <c r="E15" s="2" t="n">
         <v>971.53</v>
       </c>
-      <c r="F15" s="2" t="n">
-        <v>51.74</v>
+      <c r="F15" s="0" t="n">
+        <v>-51.74</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>2.29</v>
@@ -626,8 +626,8 @@
       <c r="E16" s="2" t="n">
         <v>962.54</v>
       </c>
-      <c r="F16" s="2" t="n">
-        <v>183.47</v>
+      <c r="F16" s="0" t="n">
+        <v>-183.47</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>171.44</v>
@@ -646,13 +646,13 @@
         <v>43362</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>942.68</v>
+        <v>962.54</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>718.22</v>
       </c>
-      <c r="F17" s="2" t="n">
-        <v>362.63</v>
+      <c r="F17" s="0" t="n">
+        <v>-362.63</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>118.22</v>
@@ -676,7 +676,7 @@
       <c r="E18" s="2" t="n">
         <v>919.35</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G18" s="2" t="n">
@@ -696,13 +696,13 @@
         <v>43364</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>848.39</v>
+        <v>919.35</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>885.33</v>
       </c>
-      <c r="F19" s="2" t="n">
-        <v>35.48</v>
+      <c r="F19" s="0" t="n">
+        <v>-35.48</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>1.44</v>
@@ -721,13 +721,13 @@
         <v>43365</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>848.99</v>
+        <v>885.33</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>867.16</v>
       </c>
-      <c r="F20" s="2" t="n">
-        <v>18.17</v>
+      <c r="F20" s="0" t="n">
+        <v>-18.17</v>
       </c>
       <c r="G20" s="2" t="n">
         <v>0</v>
@@ -746,13 +746,13 @@
         <v>43366</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>533.82</v>
+        <v>867.16</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>700.49</v>
       </c>
-      <c r="F21" s="2" t="n">
-        <v>166.67</v>
+      <c r="F21" s="0" t="n">
+        <v>-166.67</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>0</v>
@@ -776,7 +776,7 @@
       <c r="E22" s="2" t="n">
         <v>840.39</v>
       </c>
-      <c r="F22" s="2" t="n">
+      <c r="F22" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G22" s="2" t="n">
@@ -801,8 +801,8 @@
       <c r="E23" s="2" t="n">
         <v>24.8</v>
       </c>
-      <c r="F23" s="2" t="n">
-        <v>880.97</v>
+      <c r="F23" s="0" t="n">
+        <v>-880.97</v>
       </c>
       <c r="G23" s="2" t="n">
         <v>64.63</v>
@@ -826,8 +826,8 @@
       <c r="E24" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F24" s="2" t="n">
-        <v>75.49</v>
+      <c r="F24" s="0" t="n">
+        <v>-75.49</v>
       </c>
       <c r="G24" s="2" t="n">
         <v>49.56</v>
@@ -851,7 +851,7 @@
       <c r="E25" s="2" t="n">
         <v>63.2</v>
       </c>
-      <c r="F25" s="2" t="n">
+      <c r="F25" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G25" s="2" t="n">
@@ -871,13 +871,13 @@
         <v>43374</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>-63.2</v>
+        <v>63.2</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>16.38</v>
       </c>
-      <c r="F26" s="2" t="n">
-        <v>63.2</v>
+      <c r="F26" s="0" t="n">
+        <v>-63.2</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>16.3</v>
@@ -896,13 +896,13 @@
         <v>43376</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>-16.36</v>
+        <v>16.38</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>183.57</v>
       </c>
-      <c r="F27" s="2" t="n">
-        <v>16.37</v>
+      <c r="F27" s="0" t="n">
+        <v>-16.37</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>180.73</v>
@@ -926,7 +926,7 @@
       <c r="E28" s="2" t="n">
         <v>285.45</v>
       </c>
-      <c r="F28" s="2" t="n">
+      <c r="F28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G28" s="2" t="n">
@@ -946,13 +946,13 @@
         <v>43378</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>168.61</v>
+        <v>285.45</v>
       </c>
       <c r="E29" s="2" t="n">
         <v>123.61</v>
       </c>
-      <c r="F29" s="2" t="n">
-        <v>161.84</v>
+      <c r="F29" s="0" t="n">
+        <v>-161.84</v>
       </c>
       <c r="G29" s="2" t="n">
         <v>0</v>
@@ -976,7 +976,7 @@
       <c r="E30" s="2" t="n">
         <v>515.4</v>
       </c>
-      <c r="F30" s="2" t="n">
+      <c r="F30" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G30" s="2" t="n">
@@ -996,13 +996,13 @@
         <v>43380</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>195.4</v>
+        <v>515.4</v>
       </c>
       <c r="E31" s="2" t="n">
         <v>120.36</v>
       </c>
-      <c r="F31" s="2" t="n">
-        <v>395.04</v>
+      <c r="F31" s="0" t="n">
+        <v>-395.04</v>
       </c>
       <c r="G31" s="2" t="n">
         <v>0</v>
@@ -1021,13 +1021,13 @@
         <v>43381</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>-120.34</v>
+        <v>120.36</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>262.99</v>
       </c>
-      <c r="F32" s="2" t="n">
-        <v>120.35</v>
+      <c r="F32" s="0" t="n">
+        <v>-120.35</v>
       </c>
       <c r="G32" s="2" t="n">
         <v>260.35</v>
@@ -1051,7 +1051,7 @@
       <c r="E33" s="2" t="n">
         <v>565.74</v>
       </c>
-      <c r="F33" s="2" t="n">
+      <c r="F33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G33" s="2" t="n">
@@ -1071,13 +1071,13 @@
         <v>43383</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>512.78</v>
+        <v>565.74</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>453.73</v>
       </c>
-      <c r="F34" s="2" t="n">
-        <v>147.74</v>
+      <c r="F34" s="0" t="n">
+        <v>-147.74</v>
       </c>
       <c r="G34" s="2" t="n">
         <v>35.48</v>
@@ -1101,8 +1101,8 @@
       <c r="E35" s="2" t="n">
         <v>572.57</v>
       </c>
-      <c r="F35" s="2" t="n">
-        <v>200.16</v>
+      <c r="F35" s="0" t="n">
+        <v>-200.16</v>
       </c>
       <c r="G35" s="2" t="n">
         <v>315.45</v>
@@ -1121,13 +1121,13 @@
         <v>43385</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>444.05</v>
+        <v>572.57</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>638.12</v>
       </c>
-      <c r="F36" s="2" t="n">
-        <v>64.26</v>
+      <c r="F36" s="0" t="n">
+        <v>-64.26</v>
       </c>
       <c r="G36" s="2" t="n">
         <v>128.48</v>
@@ -1151,7 +1151,7 @@
       <c r="E37" s="2" t="n">
         <v>929.19</v>
       </c>
-      <c r="F37" s="2" t="n">
+      <c r="F37" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G37" s="2" t="n">
@@ -1171,13 +1171,13 @@
         <v>43387</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>861.19</v>
+        <v>929.19</v>
       </c>
       <c r="E38" s="2" t="n">
         <v>895.19</v>
       </c>
-      <c r="F38" s="2" t="n">
-        <v>34</v>
+      <c r="F38" s="0" t="n">
+        <v>-34</v>
       </c>
       <c r="G38" s="2" t="n">
         <v>0</v>
@@ -1196,13 +1196,13 @@
         <v>43388</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>847.89</v>
+        <v>895.19</v>
       </c>
       <c r="E39" s="2" t="n">
         <v>1224.77</v>
       </c>
-      <c r="F39" s="2" t="n">
-        <v>54.32</v>
+      <c r="F39" s="0" t="n">
+        <v>-54.32</v>
       </c>
       <c r="G39" s="2" t="n">
         <v>380.97</v>
@@ -1221,13 +1221,13 @@
         <v>43389</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>1065.53</v>
+        <v>1224.77</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>1263.46</v>
       </c>
-      <c r="F40" s="2" t="n">
-        <v>79.62</v>
+      <c r="F40" s="0" t="n">
+        <v>-79.62</v>
       </c>
       <c r="G40" s="2" t="n">
         <v>116.99</v>
@@ -1246,13 +1246,13 @@
         <v>43390</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>1122.12</v>
+        <v>1263.46</v>
       </c>
       <c r="E41" s="2" t="n">
         <v>1192.79</v>
       </c>
-      <c r="F41" s="2" t="n">
-        <v>70.67</v>
+      <c r="F41" s="0" t="n">
+        <v>-70.67</v>
       </c>
       <c r="G41" s="2" t="n">
         <v>0</v>
@@ -1276,8 +1276,8 @@
       <c r="E42" s="2" t="n">
         <v>738.56</v>
       </c>
-      <c r="F42" s="2" t="n">
-        <v>457.39</v>
+      <c r="F42" s="0" t="n">
+        <v>-457.39</v>
       </c>
       <c r="G42" s="2" t="n">
         <v>3.11</v>
@@ -1296,13 +1296,13 @@
         <v>43393</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>388.56</v>
+        <v>738.56</v>
       </c>
       <c r="E43" s="2" t="n">
         <v>497.96</v>
       </c>
-      <c r="F43" s="2" t="n">
-        <v>267.05</v>
+      <c r="F43" s="0" t="n">
+        <v>-267.05</v>
       </c>
       <c r="G43" s="2" t="n">
         <v>26.13</v>
@@ -1321,13 +1321,13 @@
         <v>43394</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>36.84</v>
+        <v>497.96</v>
       </c>
       <c r="E44" s="2" t="n">
         <v>453.26</v>
       </c>
-      <c r="F44" s="2" t="n">
-        <v>230.56</v>
+      <c r="F44" s="0" t="n">
+        <v>-230.56</v>
       </c>
       <c r="G44" s="2" t="n">
         <v>181.68</v>
@@ -1351,8 +1351,8 @@
       <c r="E45" s="2" t="n">
         <v>422.72</v>
       </c>
-      <c r="F45" s="2" t="n">
-        <v>47.6</v>
+      <c r="F45" s="0" t="n">
+        <v>-47.6</v>
       </c>
       <c r="G45" s="2" t="n">
         <v>17.04</v>
@@ -1371,13 +1371,13 @@
         <v>43396</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>-221.38</v>
+        <v>422.72</v>
       </c>
       <c r="E46" s="2" t="n">
         <v>261.66</v>
       </c>
-      <c r="F46" s="2" t="n">
-        <v>322.05</v>
+      <c r="F46" s="0" t="n">
+        <v>-322.05</v>
       </c>
       <c r="G46" s="2" t="n">
         <v>160</v>
@@ -1396,13 +1396,13 @@
         <v>43398</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>-146.58</v>
+        <v>261.66</v>
       </c>
       <c r="E47" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F47" s="2" t="n">
-        <v>261.65</v>
+      <c r="F47" s="0" t="n">
+        <v>-261.65</v>
       </c>
       <c r="G47" s="2" t="n">
         <v>0</v>
@@ -1426,8 +1426,8 @@
       <c r="E48" s="2" t="n">
         <v>9.97</v>
       </c>
-      <c r="F48" s="2" t="n">
-        <v>14.51</v>
+      <c r="F48" s="0" t="n">
+        <v>-14.51</v>
       </c>
       <c r="G48" s="2" t="n">
         <v>23.92</v>
@@ -1451,7 +1451,7 @@
       <c r="E49" s="2" t="n">
         <v>172.97</v>
       </c>
-      <c r="F49" s="2" t="n">
+      <c r="F49" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G49" s="2" t="n">
@@ -1471,13 +1471,13 @@
         <v>43402</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>-84.39</v>
+        <v>172.97</v>
       </c>
       <c r="E50" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F50" s="2" t="n">
-        <v>172.97</v>
+      <c r="F50" s="0" t="n">
+        <v>-172.97</v>
       </c>
       <c r="G50" s="2" t="n">
         <v>0</v>
@@ -1501,7 +1501,7 @@
       <c r="E51" s="2" t="n">
         <v>59.1</v>
       </c>
-      <c r="F51" s="2" t="n">
+      <c r="F51" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G51" s="2" t="n">
@@ -1521,13 +1521,13 @@
         <v>43409</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>11.26</v>
+        <v>59.1</v>
       </c>
       <c r="E52" s="2" t="n">
         <v>35.18</v>
       </c>
-      <c r="F52" s="2" t="n">
-        <v>23.92</v>
+      <c r="F52" s="0" t="n">
+        <v>-23.92</v>
       </c>
       <c r="G52" s="2" t="n">
         <v>0</v>
@@ -1551,7 +1551,7 @@
       <c r="E53" s="2" t="n">
         <v>139.86</v>
       </c>
-      <c r="F53" s="2" t="n">
+      <c r="F53" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G53" s="2" t="n">
@@ -1576,7 +1576,7 @@
       <c r="E54" s="2" t="n">
         <v>242.67</v>
       </c>
-      <c r="F54" s="2" t="n">
+      <c r="F54" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G54" s="2" t="n">
@@ -1596,13 +1596,13 @@
         <v>43412</v>
       </c>
       <c r="D55" s="2" t="n">
-        <v>-240.65</v>
+        <v>242.67</v>
       </c>
       <c r="E55" s="2" t="n">
         <v>1.01</v>
       </c>
-      <c r="F55" s="2" t="n">
-        <v>241.66</v>
+      <c r="F55" s="0" t="n">
+        <v>-241.66</v>
       </c>
       <c r="G55" s="2" t="n">
         <v>0</v>
@@ -1621,13 +1621,13 @@
         <v>43413</v>
       </c>
       <c r="D56" s="2" t="n">
-        <v>-0.99</v>
+        <v>1.01</v>
       </c>
       <c r="E56" s="2" t="n">
         <v>238.02</v>
       </c>
-      <c r="F56" s="2" t="n">
-        <v>1</v>
+      <c r="F56" s="0" t="n">
+        <v>-1</v>
       </c>
       <c r="G56" s="2" t="n">
         <v>235.04</v>
@@ -1646,13 +1646,13 @@
         <v>43414</v>
       </c>
       <c r="D57" s="2" t="n">
-        <v>-15.08</v>
+        <v>238.02</v>
       </c>
       <c r="E57" s="2" t="n">
         <v>229.26</v>
       </c>
-      <c r="F57" s="2" t="n">
-        <v>272.37</v>
+      <c r="F57" s="0" t="n">
+        <v>-272.37</v>
       </c>
       <c r="G57" s="2" t="n">
         <v>260.64</v>
@@ -1671,13 +1671,13 @@
         <v>43415</v>
       </c>
       <c r="D58" s="2" t="n">
-        <v>219.26</v>
+        <v>229.26</v>
       </c>
       <c r="E58" s="2" t="n">
         <v>117.43</v>
       </c>
-      <c r="F58" s="2" t="n">
-        <v>111.83</v>
+      <c r="F58" s="0" t="n">
+        <v>-111.83</v>
       </c>
       <c r="G58" s="2" t="n">
         <v>0</v>
@@ -1696,13 +1696,13 @@
         <v>43416</v>
       </c>
       <c r="D59" s="2" t="n">
-        <v>-117.43</v>
+        <v>117.43</v>
       </c>
       <c r="E59" s="2" t="n">
         <v>103.32</v>
       </c>
-      <c r="F59" s="2" t="n">
-        <v>184.46</v>
+      <c r="F59" s="0" t="n">
+        <v>-184.46</v>
       </c>
       <c r="G59" s="2" t="n">
         <v>166.88</v>
@@ -1726,8 +1726,8 @@
       <c r="E60" s="2" t="n">
         <v>65.06</v>
       </c>
-      <c r="F60" s="2" t="n">
-        <v>109.61</v>
+      <c r="F60" s="0" t="n">
+        <v>-109.61</v>
       </c>
       <c r="G60" s="2" t="n">
         <v>70.52</v>
@@ -1746,13 +1746,13 @@
         <v>43418</v>
       </c>
       <c r="D61" s="2" t="n">
-        <v>-20.58</v>
+        <v>65.06</v>
       </c>
       <c r="E61" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F61" s="2" t="n">
-        <v>65.05</v>
+      <c r="F61" s="0" t="n">
+        <v>-65.05</v>
       </c>
       <c r="G61" s="2" t="n">
         <v>0</v>
@@ -1776,8 +1776,8 @@
       <c r="E62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F62" s="2" t="n">
-        <v>23.93</v>
+      <c r="F62" s="0" t="n">
+        <v>-23.93</v>
       </c>
       <c r="G62" s="2" t="n">
         <v>23.65</v>
@@ -1801,7 +1801,7 @@
       <c r="E63" s="2" t="n">
         <v>108.3</v>
       </c>
-      <c r="F63" s="2" t="n">
+      <c r="F63" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G63" s="2" t="n">
@@ -1826,7 +1826,7 @@
       <c r="E64" s="2" t="n">
         <v>445.38</v>
       </c>
-      <c r="F64" s="2" t="n">
+      <c r="F64" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G64" s="2" t="n">
@@ -1846,13 +1846,13 @@
         <v>43424</v>
       </c>
       <c r="D65" s="2" t="n">
-        <v>-445.36</v>
+        <v>445.38</v>
       </c>
       <c r="E65" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F65" s="2" t="n">
-        <v>445.37</v>
+      <c r="F65" s="0" t="n">
+        <v>-445.37</v>
       </c>
       <c r="G65" s="2" t="n">
         <v>0</v>
@@ -1876,8 +1876,8 @@
       <c r="E66" s="2" t="n">
         <v>129.82</v>
       </c>
-      <c r="F66" s="2" t="n">
-        <v>48.15</v>
+      <c r="F66" s="0" t="n">
+        <v>-48.15</v>
       </c>
       <c r="G66" s="2" t="n">
         <v>176.28</v>
@@ -1896,13 +1896,13 @@
         <v>43426</v>
       </c>
       <c r="D67" s="2" t="n">
-        <v>-129.8</v>
+        <v>129.82</v>
       </c>
       <c r="E67" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F67" s="2" t="n">
-        <v>455.57</v>
+      <c r="F67" s="0" t="n">
+        <v>-455.57</v>
       </c>
       <c r="G67" s="2" t="n">
         <v>322.05</v>
@@ -1926,8 +1926,8 @@
       <c r="E68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F68" s="2" t="n">
-        <v>111.79</v>
+      <c r="F68" s="0" t="n">
+        <v>-111.79</v>
       </c>
       <c r="G68" s="2" t="n">
         <v>109.84</v>
@@ -1951,8 +1951,8 @@
       <c r="E69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F69" s="2" t="n">
-        <v>172.29</v>
+      <c r="F69" s="0" t="n">
+        <v>-172.29</v>
       </c>
       <c r="G69" s="2" t="n">
         <v>170.84</v>
@@ -1976,8 +1976,8 @@
       <c r="E70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F70" s="2" t="n">
-        <v>107.73</v>
+      <c r="F70" s="0" t="n">
+        <v>-107.73</v>
       </c>
       <c r="G70" s="2" t="n">
         <v>106.83</v>
@@ -2001,8 +2001,8 @@
       <c r="E71" s="2" t="n">
         <v>23.18</v>
       </c>
-      <c r="F71" s="2" t="n">
-        <v>179.12</v>
+      <c r="F71" s="0" t="n">
+        <v>-179.12</v>
       </c>
       <c r="G71" s="2" t="n">
         <v>200.48</v>
@@ -2021,13 +2021,13 @@
         <v>43439</v>
       </c>
       <c r="D72" s="2" t="n">
-        <v>-23.16</v>
+        <v>23.18</v>
       </c>
       <c r="E72" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F72" s="2" t="n">
-        <v>178.04</v>
+      <c r="F72" s="0" t="n">
+        <v>-178.04</v>
       </c>
       <c r="G72" s="2" t="n">
         <v>153.27</v>
@@ -2051,8 +2051,8 @@
       <c r="E73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F73" s="2" t="n">
-        <v>34.76</v>
+      <c r="F73" s="0" t="n">
+        <v>-34.76</v>
       </c>
       <c r="G73" s="2" t="n">
         <v>34.72</v>
@@ -2076,8 +2076,8 @@
       <c r="E74" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F74" s="2" t="n">
-        <v>56.07</v>
+      <c r="F74" s="0" t="n">
+        <v>-56.07</v>
       </c>
       <c r="G74" s="2" t="n">
         <v>55.87</v>
@@ -2101,8 +2101,8 @@
       <c r="E75" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F75" s="2" t="n">
-        <v>34.93</v>
+      <c r="F75" s="0" t="n">
+        <v>-34.93</v>
       </c>
       <c r="G75" s="2" t="n">
         <v>34.83</v>
@@ -2126,8 +2126,8 @@
       <c r="E76" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F76" s="2" t="n">
-        <v>26.24</v>
+      <c r="F76" s="0" t="n">
+        <v>-26.24</v>
       </c>
       <c r="G76" s="2" t="n">
         <v>26</v>
@@ -2151,8 +2151,8 @@
       <c r="E77" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F77" s="2" t="n">
-        <v>160.04</v>
+      <c r="F77" s="0" t="n">
+        <v>-160.04</v>
       </c>
       <c r="G77" s="2" t="n">
         <v>158.54</v>
@@ -2176,8 +2176,8 @@
       <c r="E78" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F78" s="2" t="n">
-        <v>448.74</v>
+      <c r="F78" s="0" t="n">
+        <v>-448.74</v>
       </c>
       <c r="G78" s="2" t="n">
         <v>445.37</v>
@@ -2201,8 +2201,8 @@
       <c r="E79" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F79" s="2" t="n">
-        <v>38.36</v>
+      <c r="F79" s="0" t="n">
+        <v>-38.36</v>
       </c>
       <c r="G79" s="2" t="n">
         <v>38.22</v>
@@ -2226,8 +2226,8 @@
       <c r="E80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F80" s="2" t="n">
-        <v>414.5</v>
+      <c r="F80" s="0" t="n">
+        <v>-414.5</v>
       </c>
       <c r="G80" s="2" t="n">
         <v>405.56</v>
@@ -2251,8 +2251,8 @@
       <c r="E81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F81" s="2" t="n">
-        <v>87.45</v>
+      <c r="F81" s="0" t="n">
+        <v>-87.45</v>
       </c>
       <c r="G81" s="2" t="n">
         <v>86.16</v>
@@ -2276,8 +2276,8 @@
       <c r="E82" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F82" s="2" t="n">
-        <v>341.79</v>
+      <c r="F82" s="0" t="n">
+        <v>-341.79</v>
       </c>
       <c r="G82" s="2" t="n">
         <v>336.03</v>
@@ -2301,8 +2301,8 @@
       <c r="E83" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F83" s="2" t="n">
-        <v>211.06</v>
+      <c r="F83" s="0" t="n">
+        <v>-211.06</v>
       </c>
       <c r="G83" s="2" t="n">
         <v>210.55</v>
@@ -2326,8 +2326,8 @@
       <c r="E84" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F84" s="2" t="n">
-        <v>8.44</v>
+      <c r="F84" s="0" t="n">
+        <v>-8.44</v>
       </c>
       <c r="G84" s="2" t="n">
         <v>8.25</v>
@@ -2351,8 +2351,8 @@
       <c r="E85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F85" s="2" t="n">
-        <v>74.18</v>
+      <c r="F85" s="0" t="n">
+        <v>-74.18</v>
       </c>
       <c r="G85" s="2" t="n">
         <v>73.96</v>
@@ -2376,8 +2376,8 @@
       <c r="E86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F86" s="2" t="n">
-        <v>50.56</v>
+      <c r="F86" s="0" t="n">
+        <v>-50.56</v>
       </c>
       <c r="G86" s="2" t="n">
         <v>49.98</v>
@@ -2401,8 +2401,8 @@
       <c r="E87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F87" s="2" t="n">
-        <v>50.94</v>
+      <c r="F87" s="0" t="n">
+        <v>-50.94</v>
       </c>
       <c r="G87" s="2" t="n">
         <v>50.83</v>
@@ -2426,8 +2426,8 @@
       <c r="E88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F88" s="2" t="n">
-        <v>82.45</v>
+      <c r="F88" s="0" t="n">
+        <v>-82.45</v>
       </c>
       <c r="G88" s="2" t="n">
         <v>81.84</v>
@@ -2451,8 +2451,8 @@
       <c r="E89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F89" s="2" t="n">
-        <v>84.6</v>
+      <c r="F89" s="0" t="n">
+        <v>-84.6</v>
       </c>
       <c r="G89" s="2" t="n">
         <v>83.71</v>
@@ -2476,8 +2476,8 @@
       <c r="E90" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="F90" s="2" t="n">
-        <v>48.78</v>
+      <c r="F90" s="0" t="n">
+        <v>-48.78</v>
       </c>
       <c r="G90" s="2" t="n">
         <v>48.72</v>
@@ -2512,7 +2512,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="D3 H1"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2525,8 +2525,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="10" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="10" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2575,7 +2575,7 @@
         <v>63.2</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>3684.29</v>
+        <v>-3684.29</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>2483.38</v>
@@ -2594,13 +2594,13 @@
         <v>13</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>-63.2</v>
+        <v>63.2</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>3181.35</v>
+        <v>-3181.35</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>3082.15</v>
@@ -2625,7 +2625,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>2267</v>
+        <v>-2267</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>2239.91</v>
@@ -2650,7 +2650,7 @@
         <v>0.01</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>2718.78</v>
+        <v>-2718.78</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>2689.72</v>
@@ -2685,7 +2685,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2742,7 +2742,7 @@
         <v>0.01</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>11851.42</v>
+        <v>-11851.42</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>10495.16</v>
@@ -2766,7 +2766,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>11851.42</v>
+        <v>-11851.42</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>10495.16</v>

</xml_diff>